<commit_message>
add column-level comments and README to Excel templates
</commit_message>
<xml_diff>
--- a/templates/excel/omts-import-example.xlsx
+++ b/templates/excel/omts-import-example.xlsx
@@ -200,6 +200,626 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>OMTS</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0">
+      <text>
+        <t>Required. ISO 8601 date (YYYY-MM-DD) when this data snapshot was produced.</t>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <t>Node ID of the organization whose perspective this file represents. Must match an id in the Organizations sheet.</t>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0">
+      <text>
+        <t>Who will see this file: internal (company only), partner (supply-chain partners), or public.</t>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0">
+      <text>
+        <t>Default data quality level: verified, reported, inferred, or estimated.</t>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0">
+      <text>
+        <t>Default description of how data was collected (e.g. "manual-review", "erp-export").</t>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0">
+      <text>
+        <t>ISO 8601 date when data was last verified.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>OMTS</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>Node ID of the first entity.</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <t>Node ID of the second entity (asserted to be the same real-world entity).</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <t>Confidence level: definite, probable, or possible.</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <t>Justification for the assertion (e.g. "LEI match", "manual review").</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment11.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>OMTS</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>ID of the node this identifier belongs to. Must match an id in any entity sheet.</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <t>Identifier scheme: lei, duns, gln, nat-reg, vat, or internal.</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <t>The identifier value.</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <t>Issuing authority. Required for nat-reg, vat, and internal schemes.</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <t>Access level: public, restricted, or confidential.</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <t>ISO 8601 date when the identifier became valid.</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <t>ISO 8601 date when the identifier expired.</t>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <t>Verification state: verified, reported, inferred, or unverified.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>OMTS</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>Graph-local identifier. Auto-generated from name if left blank.</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <t>Required. Legal name of the organization.</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <t>ISO 3166-1 alpha-2 country code of incorporation.</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <t>Organization lifecycle: active, dissolved, merged, or suspended.</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <t>Legal Entity Identifier (20 characters, ISO 17442).</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <t>D-U-N-S Number (9 digits).</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <t>National business registry number (e.g. Companies House number).</t>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <t>GLEIF Registration Authority code (e.g. RA000585 for UK Companies House).</t>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <t>VAT or tax identification number.</t>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <t>ISO 3166-1 alpha-2 country that issued the VAT number.</t>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <t>Your internal system identifier (e.g. SAP vendor number).</t>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <t>Name of the internal system (e.g. "sap-mm-prod").</t>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <t>General risk classification: critical, high, medium, or low.</t>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <t>Kraljic portfolio classification: strategic, leverage, bottleneck, or non-critical.</t>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0">
+      <text>
+        <t>Supplier approval status: approved, conditional, pending, blocked, or phase-out.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>OMTS</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>Graph-local identifier. Auto-generated from name if blank.</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <t>Required. Name of the facility (e.g. "Sheffield Plant").</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <t>ID of the organization that operates this facility. Must match an id in Organizations.</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <t>Street address or location description.</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <t>WGS 84 latitude (decimal degrees, e.g. 53.3811).</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <t>WGS 84 longitude (decimal degrees, e.g. -1.4701).</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <t>Global Location Number (13 digits, GS1).</t>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <t>Your internal site identifier.</t>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <t>Name of the internal system.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>OMTS</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>Graph-local identifier. Auto-generated from name if blank.</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <t>Required. Name of the product or material.</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <t>HS or CN commodity code (e.g. 7318.15 for bolts).</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <t>Unit of measure (e.g. kg, mt, pcs).</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <t>Global Trade Item Number (GS1).</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>OMTS</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>Graph-local identifier. Auto-generated if blank.</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <t>Required. Name of the certification or audit.</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <t>Required. Type: certification, audit, due_diligence_statement, self_declaration, or other.</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <t>Standard or scheme (e.g. SA8000:2014, ISO 14001).</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <t>Name of the issuing body.</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <t>Required. ISO 8601 date (YYYY-MM-DD) when the attestation takes effect.</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <t>ISO 8601 date when the attestation expires.</t>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <t>Result: pass, conditional_pass, fail, pending, or not_applicable.</t>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <t>Lifecycle: active, suspended, revoked, expired, or withdrawn.</t>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <t>External reference number or URL.</t>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <t>Risk severity: critical, high, medium, or low.</t>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <t>Risk likelihood: very_likely, likely, possible, or unlikely.</t>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <t>Node ID of the entity this attestation covers. Creates an attested_by edge.</t>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <t>Scope of the attestation (e.g. "working conditions", "environmental compliance").</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>OMTS</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>Graph-local identifier. Auto-generated if blank.</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <t>Required. Full name of the individual.</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <t>ISO 3166-1 alpha-2 country of residence.</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <t>Role description (e.g. "Director", "UBO").</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <t>ISO 3166-1 alpha-2 nationality.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>OMTS</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>Graph-local identifier. Auto-generated if blank.</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <t>Required. Description of the consignment or batch.</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <t>Lot or batch identifier.</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <t>Quantity in the consignment.</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <t>Unit of measure (e.g. kg, mt).</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <t>ISO 8601 date of production.</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <t>ISO 3166-1 alpha-2 country of origin.</t>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <t>ID of the producing facility. Must match an id in Facilities.</t>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <t>Direct (Scope 1) emissions in tonnes CO2e (CBAM).</t>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <t>Indirect (Scope 2) emissions in tonnes CO2e (CBAM).</t>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <t>Source of emissions data: actual, default_eu, or default_country.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>OMTS</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>Edge identifier. Auto-generated if blank.</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <t>Required. Relationship type: supplies, subcontracts, tolls, distributes, brokers, sells_to, operates, produces, composed_of.</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <t>Required. Source node ID (the supplier, operator, or facility).</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <t>Required. Target node ID (the buyer, facility, or good).</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <t>Required. ISO 8601 date when the relationship started.</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <t>ISO 8601 date when the relationship ended.</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <t>HS/CN code or description of what is supplied.</t>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <t>Supply-chain tier relative to the reporting entity (1 = direct).</t>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <t>Quantity supplied.</t>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <t>Unit for volume (e.g. kg, mt, pcs).</t>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <t>Annual monetary value of the relationship.</t>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <t>ISO 4217 currency code.</t>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <t>Contract or agreement reference number.</t>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <t>Percentage of buyer's demand met by this supplier (0-100).</t>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0">
+      <text>
+        <t>For distributes edges only: warehousing, transport, fulfillment, or other.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>OMTS</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>Edge identifier. Auto-generated if blank.</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <t>Required. Relationship: ownership, legal_parentage, operational_control, or beneficial_ownership.</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <t>Required. The child/subsidiary entity node ID.</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <t>Required. The parent entity node ID.</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <t>Required. ISO 8601 date when the relationship started.</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <t>ISO 8601 date when the relationship ended.</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <t>Ownership or control percentage (0-100). For ownership and beneficial_ownership.</t>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <t>TRUE for direct relationships, FALSE for indirect.</t>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <t>Type of control (for operational_control or beneficial_ownership).</t>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <t>Accounting consolidation basis (for legal_parentage): ifrs10, us_gaap_asc810, other, unknown.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1129,6 +1749,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -1182,6 +1803,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -1336,6 +1958,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -1487,6 +2110,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -1724,6 +2348,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -1825,6 +2450,7 @@
   </sheetData>
   <autoFilter ref="A1:I1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -1896,6 +2522,7 @@
   </sheetData>
   <autoFilter ref="A1:E1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -2078,6 +2705,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -2132,6 +2760,7 @@
   </sheetData>
   <autoFilter ref="A1:E1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -2227,6 +2856,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -2438,5 +3068,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>